<commit_message>
segundo commit. avances sobre vehiculos y servicio
</commit_message>
<xml_diff>
--- a/cam_base/security/generador_permisos.xlsx
+++ b/cam_base/security/generador_permisos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
   <si>
     <t>access_vehicle_for_administrator</t>
   </si>
@@ -117,28 +117,28 @@
     <t>config</t>
   </si>
   <si>
-    <t>cam_vehicle</t>
-  </si>
-  <si>
-    <t>cam_vehicle_model</t>
-  </si>
-  <si>
-    <t>cam_tool</t>
-  </si>
-  <si>
-    <t>cam_tool_model</t>
-  </si>
-  <si>
     <t>cam_out_of_service_reason</t>
   </si>
   <si>
-    <t>cam_maintainable_object</t>
-  </si>
-  <si>
-    <t>cam_engine</t>
-  </si>
-  <si>
-    <t>cam_brand</t>
+    <t>cam_elapsed_time</t>
+  </si>
+  <si>
+    <t>cam_task</t>
+  </si>
+  <si>
+    <t>cam_predefined_service</t>
+  </si>
+  <si>
+    <t>cam_service</t>
+  </si>
+  <si>
+    <t>cam_workshop</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>cam_item_task</t>
   </si>
 </sst>
 </file>
@@ -480,12 +480,12 @@
   <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" customWidth="1"/>
     <col min="4" max="4" width="39.28515625" customWidth="1"/>
     <col min="5" max="5" width="50.7109375" customWidth="1"/>
@@ -615,32 +615,32 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E7" t="str">
         <f>CONCATENATE(Datos!A2,",",Datos!B2,",",Datos!C2,",",Datos!D2,",",Datos!E2,",",Datos!F2,",",Datos!G2,",",Datos!H2)</f>
-        <v>access_cam_vehicle_for_group_name_vehicle,cam_vehicle_for_vehicle,model_cam_vehicle,group_name_vehicle,1,1,1,1</v>
+        <v>access_cam_elapsed_time_for_group_name_service,cam_elapsed_time_for_service,model_cam_elapsed_time,group_name_service,1,1,1,1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E8" t="str">
         <f>CONCATENATE(Datos!A3,",",Datos!B3,",",Datos!C3,",",Datos!D3,",",Datos!E3,",",Datos!F3,",",Datos!G3,",",Datos!H3)</f>
-        <v>access_cam_vehicle_model_for_group_name_vehicle,cam_vehicle_model_for_vehicle,model_cam_vehicle_model,group_name_vehicle,1,1,1,1</v>
+        <v>access_cam_item_task_for_group_name_service,cam_item_task_for_service,model_cam_item_task,group_name_service,1,1,1,1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -651,86 +651,83 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E9" t="str">
         <f>CONCATENATE(Datos!A4,",",Datos!B4,",",Datos!C4,",",Datos!D4,",",Datos!E4,",",Datos!F4,",",Datos!G4,",",Datos!H4)</f>
-        <v>access_cam_tool_for_group_name_vehicle,cam_tool_for_vehicle,model_cam_tool,group_name_vehicle,1,1,1,1</v>
+        <v>access_cam_task_for_group_name_service,cam_task_for_service,model_cam_task,group_name_service,1,1,1,1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
       <c r="C10" t="s">
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E10" t="str">
         <f>CONCATENATE(Datos!A5,",",Datos!B5,",",Datos!C5,",",Datos!D5,",",Datos!E5,",",Datos!F5,",",Datos!G5,",",Datos!H5)</f>
-        <v>access_cam_tool_model_for_group_name_vehicle,cam_tool_model_for_vehicle,model_cam_tool_model,group_name_vehicle,1,1,1,1</v>
+        <v>access__for_group_name_service,_for_service,model_,group_name_service,1,1,1,1</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E11" t="str">
         <f>CONCATENATE(Datos!A6,",",Datos!B6,",",Datos!C6,",",Datos!D6,",",Datos!E6,",",Datos!F6,",",Datos!G6,",",Datos!H6)</f>
-        <v>access_cam_out_of_service_reason_for_group_name_vehicle,cam_out_of_service_reason_for_vehicle,model_cam_out_of_service_reason,group_name_vehicle,1,1,1,1</v>
+        <v>access_cam_out_of_service_reason_for_group_name_service,cam_out_of_service_reason_for_service,model_cam_out_of_service_reason,group_name_service,1,1,1,1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E12" t="str">
         <f>CONCATENATE(Datos!A7,",",Datos!B7,",",Datos!C7,",",Datos!D7,",",Datos!E7,",",Datos!F7,",",Datos!G7,",",Datos!H7)</f>
-        <v>access_cam_maintainable_object_for_group_name_vehicle,cam_maintainable_object_for_vehicle,model_cam_maintainable_object,group_name_vehicle,1,1,1,1</v>
+        <v>access_cam_predefined_service_for_group_name_service,cam_predefined_service_for_service,model_cam_predefined_service,group_name_service,1,1,1,1</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E13" t="str">
         <f>CONCATENATE(Datos!A8,",",Datos!B8,",",Datos!C8,",",Datos!D8,",",Datos!E8,",",Datos!F8,",",Datos!G8,",",Datos!H8)</f>
-        <v>access_cam_engine_for_group_name_vehicle,cam_engine_for_vehicle,model_cam_engine,group_name_vehicle,1,1,1,1</v>
+        <v>access_cam_service_for_group_name_service,cam_service_for_service,model_cam_service,group_name_service,1,1,1,1</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E14" t="str">
         <f>CONCATENATE(Datos!A9,",",Datos!B9,",",Datos!C9,",",Datos!D9,",",Datos!E9,",",Datos!F9,",",Datos!G9,",",Datos!H9)</f>
-        <v>access_cam_brand_for_group_name_vehicle,cam_brand_for_vehicle,model_cam_brand,group_name_vehicle,1,1,1,1</v>
+        <v>access_cam_workshop_for_group_name_service,cam_workshop_for_service,model_cam_workshop,group_name_service,1,1,1,1</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1091,19 +1088,19 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE("access_",Permisos!B7,"_for_","group_name_",Permisos!D7)</f>
-        <v>access_cam_vehicle_for_group_name_vehicle</v>
+        <v>access_cam_elapsed_time_for_group_name_service</v>
       </c>
       <c r="B2" t="str">
         <f>CONCATENATE(Permisos!B7,"_for_",Permisos!D7)</f>
-        <v>cam_vehicle_for_vehicle</v>
+        <v>cam_elapsed_time_for_service</v>
       </c>
       <c r="C2" t="str">
         <f>CONCATENATE("model_",Permisos!B7)</f>
-        <v>model_cam_vehicle</v>
+        <v>model_cam_elapsed_time</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE("group_name_",Permisos!D7)</f>
-        <v>group_name_vehicle</v>
+        <v>group_name_service</v>
       </c>
       <c r="E2" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C7)),"1","0")</f>
@@ -1125,19 +1122,19 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE("access_",Permisos!B8,"_for_","group_name_",Permisos!D8)</f>
-        <v>access_cam_vehicle_model_for_group_name_vehicle</v>
+        <v>access_cam_item_task_for_group_name_service</v>
       </c>
       <c r="B3" t="str">
         <f>CONCATENATE(Permisos!B8,"_for_",Permisos!D8)</f>
-        <v>cam_vehicle_model_for_vehicle</v>
+        <v>cam_item_task_for_service</v>
       </c>
       <c r="C3" t="str">
         <f>CONCATENATE("model_",Permisos!B8)</f>
-        <v>model_cam_vehicle_model</v>
+        <v>model_cam_item_task</v>
       </c>
       <c r="D3" t="str">
         <f>CONCATENATE("group_name_",Permisos!D8)</f>
-        <v>group_name_vehicle</v>
+        <v>group_name_service</v>
       </c>
       <c r="E3" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C8)),"1","0")</f>
@@ -1159,19 +1156,19 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>CONCATENATE("access_",Permisos!B9,"_for_","group_name_",Permisos!D9)</f>
-        <v>access_cam_tool_for_group_name_vehicle</v>
+        <v>access_cam_task_for_group_name_service</v>
       </c>
       <c r="B4" t="str">
         <f>CONCATENATE(Permisos!B9,"_for_",Permisos!D9)</f>
-        <v>cam_tool_for_vehicle</v>
+        <v>cam_task_for_service</v>
       </c>
       <c r="C4" t="str">
         <f>CONCATENATE("model_",Permisos!B9)</f>
-        <v>model_cam_tool</v>
+        <v>model_cam_task</v>
       </c>
       <c r="D4" t="str">
         <f>CONCATENATE("group_name_",Permisos!D9)</f>
-        <v>group_name_vehicle</v>
+        <v>group_name_service</v>
       </c>
       <c r="E4" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C9)),"1","0")</f>
@@ -1193,19 +1190,19 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>CONCATENATE("access_",Permisos!B10,"_for_","group_name_",Permisos!D10)</f>
-        <v>access_cam_tool_model_for_group_name_vehicle</v>
+        <v>access__for_group_name_service</v>
       </c>
       <c r="B5" t="str">
         <f>CONCATENATE(Permisos!B10,"_for_",Permisos!D10)</f>
-        <v>cam_tool_model_for_vehicle</v>
+        <v>_for_service</v>
       </c>
       <c r="C5" t="str">
         <f>CONCATENATE("model_",Permisos!B10)</f>
-        <v>model_cam_tool_model</v>
+        <v>model_</v>
       </c>
       <c r="D5" t="str">
         <f>CONCATENATE("group_name_",Permisos!D10)</f>
-        <v>group_name_vehicle</v>
+        <v>group_name_service</v>
       </c>
       <c r="E5" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C10)),"1","0")</f>
@@ -1227,11 +1224,11 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>CONCATENATE("access_",Permisos!B11,"_for_","group_name_",Permisos!D11)</f>
-        <v>access_cam_out_of_service_reason_for_group_name_vehicle</v>
+        <v>access_cam_out_of_service_reason_for_group_name_service</v>
       </c>
       <c r="B6" t="str">
         <f>CONCATENATE(Permisos!B11,"_for_",Permisos!D11)</f>
-        <v>cam_out_of_service_reason_for_vehicle</v>
+        <v>cam_out_of_service_reason_for_service</v>
       </c>
       <c r="C6" t="str">
         <f>CONCATENATE("model_",Permisos!B11)</f>
@@ -1239,7 +1236,7 @@
       </c>
       <c r="D6" t="str">
         <f>CONCATENATE("group_name_",Permisos!D11)</f>
-        <v>group_name_vehicle</v>
+        <v>group_name_service</v>
       </c>
       <c r="E6" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C11)),"1","0")</f>
@@ -1261,19 +1258,19 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>CONCATENATE("access_",Permisos!B12,"_for_","group_name_",Permisos!D12)</f>
-        <v>access_cam_maintainable_object_for_group_name_vehicle</v>
+        <v>access_cam_predefined_service_for_group_name_service</v>
       </c>
       <c r="B7" t="str">
         <f>CONCATENATE(Permisos!B12,"_for_",Permisos!D12)</f>
-        <v>cam_maintainable_object_for_vehicle</v>
+        <v>cam_predefined_service_for_service</v>
       </c>
       <c r="C7" t="str">
         <f>CONCATENATE("model_",Permisos!B12)</f>
-        <v>model_cam_maintainable_object</v>
+        <v>model_cam_predefined_service</v>
       </c>
       <c r="D7" t="str">
         <f>CONCATENATE("group_name_",Permisos!D12)</f>
-        <v>group_name_vehicle</v>
+        <v>group_name_service</v>
       </c>
       <c r="E7" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C12)),"1","0")</f>
@@ -1295,19 +1292,19 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>CONCATENATE("access_",Permisos!B13,"_for_","group_name_",Permisos!D13)</f>
-        <v>access_cam_engine_for_group_name_vehicle</v>
+        <v>access_cam_service_for_group_name_service</v>
       </c>
       <c r="B8" t="str">
         <f>CONCATENATE(Permisos!B13,"_for_",Permisos!D13)</f>
-        <v>cam_engine_for_vehicle</v>
+        <v>cam_service_for_service</v>
       </c>
       <c r="C8" t="str">
         <f>CONCATENATE("model_",Permisos!B13)</f>
-        <v>model_cam_engine</v>
+        <v>model_cam_service</v>
       </c>
       <c r="D8" t="str">
         <f>CONCATENATE("group_name_",Permisos!D13)</f>
-        <v>group_name_vehicle</v>
+        <v>group_name_service</v>
       </c>
       <c r="E8" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C13)),"1","0")</f>
@@ -1329,19 +1326,19 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>CONCATENATE("access_",Permisos!B14,"_for_","group_name_",Permisos!D14)</f>
-        <v>access_cam_brand_for_group_name_vehicle</v>
+        <v>access_cam_workshop_for_group_name_service</v>
       </c>
       <c r="B9" t="str">
         <f>CONCATENATE(Permisos!B14,"_for_",Permisos!D14)</f>
-        <v>cam_brand_for_vehicle</v>
+        <v>cam_workshop_for_service</v>
       </c>
       <c r="C9" t="str">
         <f>CONCATENATE("model_",Permisos!B14)</f>
-        <v>model_cam_brand</v>
+        <v>model_cam_workshop</v>
       </c>
       <c r="D9" t="str">
         <f>CONCATENATE("group_name_",Permisos!D14)</f>
-        <v>group_name_vehicle</v>
+        <v>group_name_service</v>
       </c>
       <c r="E9" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C14)),"1","0")</f>

</xml_diff>